<commit_message>
Fix: export acitvity report
</commit_message>
<xml_diff>
--- a/docs/template.xlsx
+++ b/docs/template.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t xml:space="preserve">DATA REKAPITULASI</t>
   </si>
@@ -24,13 +24,13 @@
     <t xml:space="preserve">DINAS KELAUTAN DAN PERIKANAN PROVINSI JAWA BARAT</t>
   </si>
   <si>
-    <t>BULAN:</t>
-  </si>
-  <si>
-    <t>TAHUN:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNIT KERJA:</t>
+    <t xml:space="preserve">Jenis Pengawasan</t>
+  </si>
+  <si>
+    <t>Kabupaten</t>
+  </si>
+  <si>
+    <t>Tahun</t>
   </si>
   <si>
     <t xml:space="preserve">Nomor (ID BAP)</t>
@@ -39,9 +39,6 @@
     <t xml:space="preserve">Nama Kegiatan</t>
   </si>
   <si>
-    <t xml:space="preserve">Jenis Pengawasan</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nama Pengawas</t>
   </si>
   <si>
@@ -109,9 +106,6 @@
   </si>
   <si>
     <t>Kecamatan</t>
-  </si>
-  <si>
-    <t>Kabupaten</t>
   </si>
   <si>
     <t>Provinsi</t>
@@ -166,8 +160,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11.000000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -182,7 +183,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -191,137 +192,17 @@
       <diagonal style="none"/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
+      <left style="thin">
+        <color theme="1"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color theme="1"/>
       </right>
-      <top style="medium">
-        <color auto="1"/>
+      <top style="thin">
+        <color theme="1"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
+        <color theme="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
@@ -329,38 +210,20 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -872,13 +735,13 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="1"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="P1" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="1" max="1" width="14"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" width="16.28125"/>
     <col bestFit="1" customWidth="1" min="2" max="2" width="13.36328125"/>
     <col bestFit="1" customWidth="1" min="3" max="3" width="15.7265625"/>
     <col bestFit="1" customWidth="1" min="4" max="4" width="14.54296875"/>
@@ -1036,625 +899,630 @@
       <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
     </row>
-    <row r="5" ht="15">
-      <c r="A5" t="s">
+    <row r="5" ht="14.25">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
+    <row r="8" ht="15"/>
+    <row r="9">
+      <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4" t="s">
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4" t="s">
+      <c r="Q9" s="4"/>
+      <c r="R9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="3" t="s">
+      <c r="S9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="T9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="U9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="U6" s="3" t="s">
+      <c r="V9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="V6" s="4" t="s">
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="3" t="s">
+      <c r="AA9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AA6" s="3" t="s">
+      <c r="AB9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AB6" s="4" t="s">
+      <c r="AC9" s="4"/>
+      <c r="AD9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AC6" s="4"/>
-      <c r="AD6" s="4" t="s">
+      <c r="AE9" s="4"/>
+      <c r="AF9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AE6" s="4"/>
-      <c r="AF6" s="4" t="s">
+      <c r="AG9" s="4"/>
+      <c r="AH9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AG6" s="4"/>
-      <c r="AH6" s="3" t="s">
+      <c r="AI9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AI6" s="3" t="s">
+      <c r="AJ9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AJ6" s="5" t="s">
+    </row>
+    <row r="10">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="8" t="s">
+      <c r="I10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="J10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="K10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="M10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="N10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="M7" s="8" t="s">
+      <c r="O10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="P10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="Q10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="P7" s="8" t="s">
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="Q7" s="8" t="s">
+      <c r="W10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="8" t="s">
+      <c r="X10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="W7" s="8" t="s">
+      <c r="Y10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="X7" s="8" t="s">
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Y7" s="8" t="s">
+      <c r="AC10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="Z7" s="7"/>
-      <c r="AA7" s="7"/>
-      <c r="AB7" s="8" t="s">
+      <c r="AD10" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AC7" s="8" t="s">
+      <c r="AE10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AD7" s="8" t="s">
+      <c r="AF10" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="AE7" s="8" t="s">
+      <c r="AG10" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="AF7" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="AG7" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH7" s="7"/>
-      <c r="AI7" s="7"/>
-      <c r="AJ7" s="9"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="10"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="8"/>
-      <c r="AA8" s="8"/>
-      <c r="AB8" s="8"/>
-      <c r="AC8" s="8"/>
-      <c r="AD8" s="8"/>
-      <c r="AE8" s="8"/>
-      <c r="AF8" s="8"/>
-      <c r="AG8" s="8"/>
-      <c r="AH8" s="8"/>
-      <c r="AI8" s="8"/>
-      <c r="AJ8" s="11"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="10"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="8"/>
-      <c r="W9" s="8"/>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="8"/>
-      <c r="Z9" s="8"/>
-      <c r="AA9" s="8"/>
-      <c r="AB9" s="8"/>
-      <c r="AC9" s="8"/>
-      <c r="AD9" s="8"/>
-      <c r="AE9" s="8"/>
-      <c r="AF9" s="8"/>
-      <c r="AG9" s="8"/>
-      <c r="AH9" s="8"/>
-      <c r="AI9" s="8"/>
-      <c r="AJ9" s="11"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="10"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
-      <c r="V10" s="8"/>
-      <c r="W10" s="8"/>
-      <c r="X10" s="8"/>
-      <c r="Y10" s="8"/>
-      <c r="Z10" s="8"/>
-      <c r="AA10" s="8"/>
-      <c r="AB10" s="8"/>
-      <c r="AC10" s="8"/>
-      <c r="AD10" s="8"/>
-      <c r="AE10" s="8"/>
-      <c r="AF10" s="8"/>
-      <c r="AG10" s="8"/>
-      <c r="AH10" s="8"/>
-      <c r="AI10" s="8"/>
-      <c r="AJ10" s="11"/>
+      <c r="AH10" s="3"/>
+      <c r="AI10" s="3"/>
+      <c r="AJ10" s="3"/>
     </row>
     <row r="11">
-      <c r="A11" s="10"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="8"/>
-      <c r="AA11" s="8"/>
-      <c r="AB11" s="8"/>
-      <c r="AC11" s="8"/>
-      <c r="AD11" s="8"/>
-      <c r="AE11" s="8"/>
-      <c r="AF11" s="8"/>
-      <c r="AG11" s="8"/>
-      <c r="AH11" s="8"/>
-      <c r="AI11" s="8"/>
-      <c r="AJ11" s="11"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="6"/>
+      <c r="AC11" s="6"/>
+      <c r="AD11" s="6"/>
+      <c r="AE11" s="6"/>
+      <c r="AF11" s="6"/>
+      <c r="AG11" s="6"/>
+      <c r="AH11" s="6"/>
+      <c r="AI11" s="6"/>
+      <c r="AJ11" s="6"/>
     </row>
     <row r="12">
-      <c r="A12" s="10"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
-      <c r="V12" s="8"/>
-      <c r="W12" s="8"/>
-      <c r="X12" s="8"/>
-      <c r="Y12" s="8"/>
-      <c r="Z12" s="8"/>
-      <c r="AA12" s="8"/>
-      <c r="AB12" s="8"/>
-      <c r="AC12" s="8"/>
-      <c r="AD12" s="8"/>
-      <c r="AE12" s="8"/>
-      <c r="AF12" s="8"/>
-      <c r="AG12" s="8"/>
-      <c r="AH12" s="8"/>
-      <c r="AI12" s="8"/>
-      <c r="AJ12" s="11"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="6"/>
+      <c r="AC12" s="6"/>
+      <c r="AD12" s="6"/>
+      <c r="AE12" s="6"/>
+      <c r="AF12" s="6"/>
+      <c r="AG12" s="6"/>
+      <c r="AH12" s="6"/>
+      <c r="AI12" s="6"/>
+      <c r="AJ12" s="6"/>
     </row>
     <row r="13">
-      <c r="A13" s="10"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="8"/>
-      <c r="Z13" s="8"/>
-      <c r="AA13" s="8"/>
-      <c r="AB13" s="8"/>
-      <c r="AC13" s="8"/>
-      <c r="AD13" s="8"/>
-      <c r="AE13" s="8"/>
-      <c r="AF13" s="8"/>
-      <c r="AG13" s="8"/>
-      <c r="AH13" s="8"/>
-      <c r="AI13" s="8"/>
-      <c r="AJ13" s="11"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="6"/>
+      <c r="AA13" s="6"/>
+      <c r="AB13" s="6"/>
+      <c r="AC13" s="6"/>
+      <c r="AD13" s="6"/>
+      <c r="AE13" s="6"/>
+      <c r="AF13" s="6"/>
+      <c r="AG13" s="6"/>
+      <c r="AH13" s="6"/>
+      <c r="AI13" s="6"/>
+      <c r="AJ13" s="6"/>
     </row>
     <row r="14">
-      <c r="A14" s="10"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="8"/>
-      <c r="W14" s="8"/>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="8"/>
-      <c r="Z14" s="8"/>
-      <c r="AA14" s="8"/>
-      <c r="AB14" s="8"/>
-      <c r="AC14" s="8"/>
-      <c r="AD14" s="8"/>
-      <c r="AE14" s="8"/>
-      <c r="AF14" s="8"/>
-      <c r="AG14" s="8"/>
-      <c r="AH14" s="8"/>
-      <c r="AI14" s="8"/>
-      <c r="AJ14" s="11"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="6"/>
+      <c r="AA14" s="6"/>
+      <c r="AB14" s="6"/>
+      <c r="AC14" s="6"/>
+      <c r="AD14" s="6"/>
+      <c r="AE14" s="6"/>
+      <c r="AF14" s="6"/>
+      <c r="AG14" s="6"/>
+      <c r="AH14" s="6"/>
+      <c r="AI14" s="6"/>
+      <c r="AJ14" s="6"/>
     </row>
     <row r="15">
-      <c r="A15" s="10"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="8"/>
-      <c r="Y15" s="8"/>
-      <c r="Z15" s="8"/>
-      <c r="AA15" s="8"/>
-      <c r="AB15" s="8"/>
-      <c r="AC15" s="8"/>
-      <c r="AD15" s="8"/>
-      <c r="AE15" s="8"/>
-      <c r="AF15" s="8"/>
-      <c r="AG15" s="8"/>
-      <c r="AH15" s="8"/>
-      <c r="AI15" s="8"/>
-      <c r="AJ15" s="11"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="6"/>
+      <c r="AE15" s="6"/>
+      <c r="AF15" s="6"/>
+      <c r="AG15" s="6"/>
+      <c r="AH15" s="6"/>
+      <c r="AI15" s="6"/>
+      <c r="AJ15" s="6"/>
     </row>
     <row r="16">
-      <c r="A16" s="10"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
-      <c r="V16" s="8"/>
-      <c r="W16" s="8"/>
-      <c r="X16" s="8"/>
-      <c r="Y16" s="8"/>
-      <c r="Z16" s="8"/>
-      <c r="AA16" s="8"/>
-      <c r="AB16" s="8"/>
-      <c r="AC16" s="8"/>
-      <c r="AD16" s="8"/>
-      <c r="AE16" s="8"/>
-      <c r="AF16" s="8"/>
-      <c r="AG16" s="8"/>
-      <c r="AH16" s="8"/>
-      <c r="AI16" s="8"/>
-      <c r="AJ16" s="11"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="6"/>
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="6"/>
+      <c r="AE16" s="6"/>
+      <c r="AF16" s="6"/>
+      <c r="AG16" s="6"/>
+      <c r="AH16" s="6"/>
+      <c r="AI16" s="6"/>
+      <c r="AJ16" s="6"/>
     </row>
     <row r="17">
-      <c r="A17" s="10"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="8"/>
-      <c r="Y17" s="8"/>
-      <c r="Z17" s="8"/>
-      <c r="AA17" s="8"/>
-      <c r="AB17" s="8"/>
-      <c r="AC17" s="8"/>
-      <c r="AD17" s="8"/>
-      <c r="AE17" s="8"/>
-      <c r="AF17" s="8"/>
-      <c r="AG17" s="8"/>
-      <c r="AH17" s="8"/>
-      <c r="AI17" s="8"/>
-      <c r="AJ17" s="11"/>
-    </row>
-    <row r="18" ht="15">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
-      <c r="V18" s="13"/>
-      <c r="W18" s="13"/>
-      <c r="X18" s="13"/>
-      <c r="Y18" s="13"/>
-      <c r="Z18" s="13"/>
-      <c r="AA18" s="13"/>
-      <c r="AB18" s="13"/>
-      <c r="AC18" s="13"/>
-      <c r="AD18" s="13"/>
-      <c r="AE18" s="13"/>
-      <c r="AF18" s="13"/>
-      <c r="AG18" s="13"/>
-      <c r="AH18" s="13"/>
-      <c r="AI18" s="13"/>
-      <c r="AJ18" s="14"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="6"/>
+      <c r="AC17" s="6"/>
+      <c r="AD17" s="6"/>
+      <c r="AE17" s="6"/>
+      <c r="AF17" s="6"/>
+      <c r="AG17" s="6"/>
+      <c r="AH17" s="6"/>
+      <c r="AI17" s="6"/>
+      <c r="AJ17" s="6"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="6"/>
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="6"/>
+      <c r="AD18" s="6"/>
+      <c r="AE18" s="6"/>
+      <c r="AF18" s="6"/>
+      <c r="AG18" s="6"/>
+      <c r="AH18" s="6"/>
+      <c r="AI18" s="6"/>
+      <c r="AJ18" s="6"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="6"/>
+      <c r="Z19" s="6"/>
+      <c r="AA19" s="6"/>
+      <c r="AB19" s="6"/>
+      <c r="AC19" s="6"/>
+      <c r="AD19" s="6"/>
+      <c r="AE19" s="6"/>
+      <c r="AF19" s="6"/>
+      <c r="AG19" s="6"/>
+      <c r="AH19" s="6"/>
+      <c r="AI19" s="6"/>
+      <c r="AJ19" s="6"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="6"/>
+      <c r="AA20" s="6"/>
+      <c r="AB20" s="6"/>
+      <c r="AC20" s="6"/>
+      <c r="AD20" s="6"/>
+      <c r="AE20" s="6"/>
+      <c r="AF20" s="6"/>
+      <c r="AG20" s="6"/>
+      <c r="AH20" s="6"/>
+      <c r="AI20" s="6"/>
+      <c r="AJ20" s="6"/>
+    </row>
+    <row r="21" ht="15">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="6"/>
+      <c r="AB21" s="6"/>
+      <c r="AC21" s="6"/>
+      <c r="AD21" s="6"/>
+      <c r="AE21" s="6"/>
+      <c r="AF21" s="6"/>
+      <c r="AG21" s="6"/>
+      <c r="AH21" s="6"/>
+      <c r="AI21" s="6"/>
+      <c r="AJ21" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="26">
     <mergeCell ref="A1:AJ1"/>
     <mergeCell ref="A2:AJ2"/>
     <mergeCell ref="A3:AJ3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="T6:T7"/>
-    <mergeCell ref="U6:U7"/>
-    <mergeCell ref="V6:Y6"/>
-    <mergeCell ref="Z6:Z7"/>
-    <mergeCell ref="AA6:AA7"/>
-    <mergeCell ref="AB6:AC6"/>
-    <mergeCell ref="AD6:AE6"/>
-    <mergeCell ref="AF6:AG6"/>
-    <mergeCell ref="AH6:AH7"/>
-    <mergeCell ref="AI6:AI7"/>
-    <mergeCell ref="AJ6:AJ7"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:L9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="V9:Y9"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AC9"/>
+    <mergeCell ref="AD9:AE9"/>
+    <mergeCell ref="AF9:AG9"/>
+    <mergeCell ref="AH9:AH10"/>
+    <mergeCell ref="AI9:AI10"/>
+    <mergeCell ref="AJ9:AJ10"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>